<commit_message>
add es test project to git
</commit_message>
<xml_diff>
--- a/ids/development environment.xlsx
+++ b/ids/development environment.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7620" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="191">
   <si>
     <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -760,6 +760,14 @@
   </si>
   <si>
     <t>google email/Mzfnnnn5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lantern</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vpn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1225,15 +1233,15 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1252,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1255,7 +1263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1266,7 +1274,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1277,7 +1285,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1288,15 +1296,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1304,7 +1312,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1312,11 +1320,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>62</v>
       </c>
@@ -1327,7 +1335,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>65</v>
       </c>
@@ -1336,7 +1344,7 @@
       </c>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>67</v>
       </c>
@@ -1345,7 +1353,7 @@
       </c>
       <c r="C17" s="17"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>69</v>
       </c>
@@ -1354,7 +1362,7 @@
       </c>
       <c r="C18" s="17"/>
     </row>
-    <row r="19" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>70</v>
       </c>
@@ -1365,7 +1373,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>73</v>
       </c>
@@ -1376,7 +1384,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>75</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>77</v>
       </c>
@@ -1396,7 +1404,7 @@
       </c>
       <c r="C22" s="17"/>
     </row>
-    <row r="23" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>79</v>
       </c>
@@ -1407,7 +1415,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>81</v>
       </c>
@@ -1433,16 +1441,16 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>155</v>
       </c>
@@ -1453,7 +1461,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -1464,7 +1472,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -1475,7 +1483,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>153</v>
       </c>
@@ -1486,7 +1494,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -1497,7 +1505,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -1508,7 +1516,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -1519,7 +1527,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -1530,7 +1538,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -1541,7 +1549,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -1552,12 +1560,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>173</v>
       </c>
@@ -1565,7 +1573,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>175</v>
       </c>
@@ -1581,41 +1589,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -1629,7 +1637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1643,7 +1651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +1665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1665,7 +1673,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -1673,12 +1681,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>103</v>
       </c>
@@ -1686,7 +1694,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>110</v>
       </c>
@@ -1697,7 +1705,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -1725,14 +1733,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1743,7 +1751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1751,7 +1759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1767,23 +1775,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="111.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="111.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -1794,7 +1802,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1802,7 +1810,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1810,7 +1818,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1818,7 +1826,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1826,7 +1834,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1837,7 +1845,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -1848,7 +1856,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -1856,12 +1864,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>126</v>
       </c>
@@ -1875,7 +1883,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>178</v>
       </c>
@@ -1883,7 +1891,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>176</v>
       </c>
@@ -1891,17 +1899,17 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>180</v>
       </c>
@@ -1912,7 +1920,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -1920,12 +1928,20 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>186</v>
       </c>
       <c r="C25" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1946,16 +1962,16 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>38</v>
       </c>
@@ -1978,7 +1994,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>42891</v>
       </c>
@@ -1995,7 +2011,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>42892</v>
       </c>
@@ -2010,7 +2026,7 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>42893</v>
       </c>
@@ -2024,7 +2040,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>42894</v>
       </c>
@@ -2032,7 +2048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>42895</v>
       </c>
@@ -2054,14 +2070,14 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -2072,7 +2088,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2086,7 +2102,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -2094,7 +2110,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>92</v>
       </c>
@@ -2123,13 +2139,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -2137,12 +2153,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -2150,7 +2166,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -2158,7 +2174,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -2183,19 +2199,19 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -2206,10 +2222,10 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" s="1"/>
     </row>
   </sheetData>
@@ -2227,9 +2243,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>131</v>
       </c>
@@ -2237,7 +2253,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -2248,7 +2264,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>135</v>
       </c>
@@ -2256,7 +2272,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -2267,17 +2283,17 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>140</v>
       </c>

</xml_diff>